<commit_message>
to double check but should work now!
</commit_message>
<xml_diff>
--- a/support/add_sectors/master.xlsx
+++ b/support/add_sectors/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/ExioSteel/support/add_sectors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62143BE-7219-6649-A59B-4578D7380C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF70D14-E5A9-924F-B804-7B309ECCDF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="51200" windowHeight="26880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -2910,8 +2910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2924,7 +2924,7 @@
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -12595,8 +12595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12752,7 +12752,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12985,13 +12985,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13203,8 +13204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13332,7 +13333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>

</xml_diff>